<commit_message>
Updated code to fix bond data issue
Updated code to fix bond data issue
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShyamPC\Documents\GitHub\auto-valuation-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShyamPC\Desktop\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D38B00-3041-4190-99A5-E50FBE7DC366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0B3429-B4E2-4B20-A48C-AFCA53FAC7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="6" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="377">
   <si>
     <t>EPS</t>
   </si>
@@ -1249,6 +1249,9 @@
   </si>
   <si>
     <t>Still need to automate:</t>
+  </si>
+  <si>
+    <t>&lt;- Use CTRL+SHIFT+ENTER if modifying</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1765,6 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -1827,6 +1829,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -2123,8 +2126,8 @@
   </sheetPr>
   <dimension ref="A1:AL34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2205,7 +2208,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="29"/>
       <c r="P3" s="36"/>
-      <c r="S3" s="67" t="s">
+      <c r="S3" s="66" t="s">
         <v>92</v>
       </c>
       <c r="T3" s="4">
@@ -2216,7 +2219,7 @@
         <v>310</v>
       </c>
       <c r="Z3">
-        <f>VLOOKUP("Short-term debt",'Balance Sheet (Annual)'!$A$1:$Z$48,2,FALSE)</f>
+        <f>_xlfn.IFNA(VLOOKUP("Short-term debt",'Balance Sheet (Annual)'!$A$1:$Z$48,2,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="AA3">
@@ -2244,10 +2247,10 @@
         <v>53</v>
       </c>
       <c r="P4" s="36"/>
-      <c r="S4" s="67" t="s">
+      <c r="S4" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="T4" s="68" t="e">
+      <c r="T4" s="67" t="e">
         <f>SUMPRODUCT('Debt Template'!C3:C2166,'Debt Template'!B3:B2166)/T3</f>
         <v>#DIV/0!</v>
       </c>
@@ -2290,10 +2293,10 @@
         <f>AVERAGE(P2:P4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S5" s="67" t="s">
+      <c r="S5" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="T5" s="66" t="e">
+      <c r="T5" s="65" t="e">
         <f>T4 * (1-P14)</f>
         <v>#DIV/0!</v>
       </c>
@@ -2386,9 +2389,9 @@
       <c r="Y8" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="Z8" s="65" t="e">
-        <f>Z7*(1-Z11)</f>
-        <v>#DIV/0!</v>
+      <c r="Z8" s="86">
+        <f>Z11*(1-P14)</f>
+        <v>0.1512</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
@@ -2486,7 +2489,7 @@
       <c r="Y11" t="s">
         <v>106</v>
       </c>
-      <c r="Z11" s="87">
+      <c r="Z11" s="86">
         <f>'Credit Ratings'!B21+DCF!P17</f>
         <v>0.1512</v>
       </c>
@@ -2755,15 +2758,15 @@
         <v>116</v>
       </c>
       <c r="G24" s="50"/>
-      <c r="H24" s="92" t="s">
+      <c r="H24" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="92"/>
-      <c r="M24" s="92"/>
-      <c r="N24" s="92"/>
+      <c r="I24" s="91"/>
+      <c r="J24" s="91"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="91"/>
+      <c r="N24" s="91"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="33" t="s">
@@ -2780,15 +2783,15 @@
       <c r="D25" s="46">
         <v>0.8</v>
       </c>
-      <c r="H25" s="91" t="s">
+      <c r="H25" s="90" t="s">
         <v>122</v>
       </c>
-      <c r="I25" s="91"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="91"/>
-      <c r="M25" s="91"/>
-      <c r="N25" s="91"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33" t="s">
@@ -2805,7 +2808,7 @@
       <c r="D26" s="46">
         <v>0.2</v>
       </c>
-      <c r="F26" s="93" t="s">
+      <c r="F26" s="92" t="s">
         <v>123</v>
       </c>
       <c r="G26" s="51" t="e">
@@ -2849,7 +2852,7 @@
       <c r="D27" s="46">
         <v>0</v>
       </c>
-      <c r="F27" s="93"/>
+      <c r="F27" s="92"/>
       <c r="G27" s="8">
         <v>5.5E-2</v>
       </c>
@@ -2892,7 +2895,7 @@
         <f>SUM(D25:D27)</f>
         <v>1</v>
       </c>
-      <c r="F28" s="93"/>
+      <c r="F28" s="92"/>
       <c r="G28" s="8">
         <v>0.06</v>
       </c>
@@ -2919,7 +2922,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="93"/>
+      <c r="F29" s="92"/>
       <c r="G29" s="8">
         <f>G28+0.005</f>
         <v>6.5000000000000002E-2</v>
@@ -2947,7 +2950,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F30" s="93"/>
+      <c r="F30" s="92"/>
       <c r="G30" s="8">
         <f t="shared" ref="G30:G33" si="3">G29+0.005</f>
         <v>7.0000000000000007E-2</v>
@@ -2975,7 +2978,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F31" s="93"/>
+      <c r="F31" s="92"/>
       <c r="G31" s="8">
         <f t="shared" si="3"/>
         <v>7.5000000000000011E-2</v>
@@ -3003,7 +3006,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F32" s="93"/>
+      <c r="F32" s="92"/>
       <c r="G32" s="8">
         <f t="shared" si="3"/>
         <v>8.0000000000000016E-2</v>
@@ -3031,7 +3034,7 @@
       </c>
     </row>
     <row r="33" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F33" s="93"/>
+      <c r="F33" s="92"/>
       <c r="G33" s="8">
         <f t="shared" si="3"/>
         <v>8.500000000000002E-2</v>
@@ -3059,7 +3062,7 @@
       </c>
     </row>
     <row r="34" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F34" s="93"/>
+      <c r="F34" s="92"/>
       <c r="G34" s="8">
         <v>0.09</v>
       </c>
@@ -13367,483 +13370,483 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="88"/>
+    <col min="5" max="5" width="8.88671875" style="87"/>
     <col min="6" max="6" width="66.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>371</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="83" t="s">
         <v>372</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="83" t="s">
         <v>337</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="83" t="s">
         <v>338</v>
       </c>
       <c r="F2" t="s">
         <v>339</v>
       </c>
-      <c r="M2" s="84" t="s">
+      <c r="M2" s="83" t="s">
         <v>337</v>
       </c>
-      <c r="N2" s="84" t="s">
+      <c r="N2" s="83" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A3" s="88">
+      <c r="A3" s="87">
         <v>-100000</v>
       </c>
-      <c r="B3" s="88">
+      <c r="B3" s="87">
         <v>0.19999900000000001</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="87" t="s">
         <v>336</v>
       </c>
-      <c r="D3" s="89">
+      <c r="D3" s="88">
         <v>0.1512</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="M3" s="85" t="s">
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="M3" s="84" t="s">
         <v>342</v>
       </c>
-      <c r="N3" s="86">
+      <c r="N3" s="85">
         <v>6.3E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88">
+    <row r="4" spans="1:30" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="87">
         <v>0.2</v>
       </c>
-      <c r="B4" s="88">
+      <c r="B4" s="87">
         <v>0.64999899999999999</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="87" t="s">
         <v>335</v>
       </c>
-      <c r="D4" s="89">
+      <c r="D4" s="88">
         <v>0.1134</v>
       </c>
-      <c r="E4" s="88"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="9"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="89"/>
-      <c r="M4" s="85" t="s">
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="88"/>
+      <c r="M4" s="84" t="s">
         <v>341</v>
       </c>
-      <c r="N4" s="86">
+      <c r="N4" s="85">
         <v>6.3E-3</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5" s="88">
+      <c r="A5" s="87">
         <v>0.65</v>
       </c>
-      <c r="B5" s="88">
+      <c r="B5" s="87">
         <v>0.79999900000000002</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="87" t="s">
         <v>334</v>
       </c>
-      <c r="D5" s="89">
+      <c r="D5" s="88">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="89"/>
-      <c r="M5" s="85" t="s">
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="88"/>
+      <c r="M5" s="84" t="s">
         <v>344</v>
       </c>
-      <c r="N5" s="86">
+      <c r="N5" s="85">
         <v>7.7999999999999996E-3</v>
       </c>
-      <c r="P5" s="88">
+      <c r="P5" s="87">
         <v>8.5</v>
       </c>
-      <c r="Q5" s="88">
+      <c r="Q5" s="87">
         <v>6.5</v>
       </c>
-      <c r="R5" s="88">
+      <c r="R5" s="87">
         <v>5.5</v>
       </c>
-      <c r="S5" s="88">
+      <c r="S5" s="87">
         <v>4.25</v>
       </c>
-      <c r="T5" s="88">
+      <c r="T5" s="87">
         <v>3</v>
       </c>
-      <c r="U5" s="88">
+      <c r="U5" s="87">
         <v>2.5</v>
       </c>
-      <c r="V5" s="88">
+      <c r="V5" s="87">
         <v>2.25</v>
       </c>
-      <c r="W5" s="88">
+      <c r="W5" s="87">
         <v>2</v>
       </c>
-      <c r="X5" s="88">
+      <c r="X5" s="87">
         <v>1.75</v>
       </c>
-      <c r="Y5" s="88">
+      <c r="Y5" s="87">
         <v>1.5</v>
       </c>
-      <c r="Z5" s="88">
+      <c r="Z5" s="87">
         <v>1.25</v>
       </c>
-      <c r="AA5" s="88">
+      <c r="AA5" s="87">
         <v>0.8</v>
       </c>
-      <c r="AB5" s="88">
+      <c r="AB5" s="87">
         <v>0.65</v>
       </c>
-      <c r="AC5" s="88">
+      <c r="AC5" s="87">
         <v>0.2</v>
       </c>
-      <c r="AD5" s="88">
+      <c r="AD5" s="87">
         <v>-100000</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="88">
+    <row r="6" spans="1:30" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="87">
         <v>0.8</v>
       </c>
-      <c r="B6" s="88">
+      <c r="B6" s="87">
         <v>1.2499990000000001</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="87" t="s">
         <v>333</v>
       </c>
-      <c r="D6" s="89">
+      <c r="D6" s="88">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="89"/>
-      <c r="M6" s="85" t="s">
+      <c r="E6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="M6" s="84" t="s">
         <v>343</v>
       </c>
-      <c r="N6" s="86">
+      <c r="N6" s="85">
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A7" s="88">
+      <c r="A7" s="87">
         <v>1.25</v>
       </c>
-      <c r="B7" s="88">
+      <c r="B7" s="87">
         <v>1.4999990000000001</v>
       </c>
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="87" t="s">
         <v>332</v>
       </c>
-      <c r="D7" s="89">
+      <c r="D7" s="88">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="89"/>
-      <c r="M7" s="85" t="s">
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="88"/>
+      <c r="M7" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="N7" s="86">
+      <c r="N7" s="85">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="88">
+    <row r="8" spans="1:30" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="87">
         <v>1.5</v>
       </c>
-      <c r="B8" s="88">
+      <c r="B8" s="87">
         <v>1.7499990000000001</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="87" t="s">
         <v>331</v>
       </c>
-      <c r="D8" s="89">
+      <c r="D8" s="88">
         <v>4.2099999999999999E-2</v>
       </c>
-      <c r="E8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
-      <c r="K8" s="89"/>
-      <c r="M8" s="85" t="s">
+      <c r="E8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="88"/>
+      <c r="M8" s="84" t="s">
         <v>345</v>
       </c>
-      <c r="N8" s="86">
+      <c r="N8" s="85">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A9" s="88">
+      <c r="A9" s="87">
         <v>1.75</v>
       </c>
-      <c r="B9" s="88">
+      <c r="B9" s="87">
         <v>1.9999990000000001</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="87" t="s">
         <v>330</v>
       </c>
-      <c r="D9" s="89">
+      <c r="D9" s="88">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="89"/>
-      <c r="M9" s="85" t="s">
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="88"/>
+      <c r="M9" s="84" t="s">
         <v>348</v>
       </c>
-      <c r="N9" s="86">
+      <c r="N9" s="85">
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="88">
+    <row r="10" spans="1:30" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="87">
         <v>2</v>
       </c>
-      <c r="B10" s="88">
+      <c r="B10" s="87">
         <v>2.2499999000000002</v>
       </c>
-      <c r="C10" s="88" t="s">
+      <c r="C10" s="87" t="s">
         <v>329</v>
       </c>
-      <c r="D10" s="89">
+      <c r="D10" s="88">
         <v>2.4E-2</v>
       </c>
-      <c r="E10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="89"/>
-      <c r="M10" s="85" t="s">
+      <c r="E10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="88"/>
+      <c r="M10" s="84" t="s">
         <v>347</v>
       </c>
-      <c r="N10" s="86">
+      <c r="N10" s="85">
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A11" s="88">
+      <c r="A11" s="87">
         <v>2.25</v>
       </c>
-      <c r="B11" s="88">
+      <c r="B11" s="87">
         <v>2.2499989999999999</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="87" t="s">
         <v>328</v>
       </c>
-      <c r="D11" s="89">
+      <c r="D11" s="88">
         <v>0.02</v>
       </c>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="89"/>
-      <c r="M11" s="85" t="s">
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="88"/>
+      <c r="M11" s="84" t="s">
         <v>350</v>
       </c>
-      <c r="N11" s="86">
+      <c r="N11" s="85">
         <v>1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="88">
+    <row r="12" spans="1:30" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="87">
         <v>2.5</v>
       </c>
-      <c r="B12" s="88">
+      <c r="B12" s="87">
         <v>2.9999989999999999</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="87" t="s">
         <v>327</v>
       </c>
-      <c r="D12" s="89">
+      <c r="D12" s="88">
         <v>1.5599999999999999E-2</v>
       </c>
-      <c r="E12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="89"/>
-      <c r="M12" s="85" t="s">
+      <c r="E12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="88"/>
+      <c r="M12" s="84" t="s">
         <v>349</v>
       </c>
-      <c r="N12" s="86">
+      <c r="N12" s="85">
         <v>1.2200000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A13" s="88">
+      <c r="A13" s="87">
         <v>3</v>
       </c>
-      <c r="B13" s="88">
+      <c r="B13" s="87">
         <v>4.2499989999999999</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="87" t="s">
         <v>326</v>
       </c>
-      <c r="D13" s="89">
+      <c r="D13" s="88">
         <v>1.2200000000000001E-2</v>
       </c>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="89"/>
-      <c r="M13" s="85" t="s">
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="88"/>
+      <c r="M13" s="84" t="s">
         <v>352</v>
       </c>
-      <c r="N13" s="86">
+      <c r="N13" s="85">
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="88">
+    <row r="14" spans="1:30" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="87">
         <v>4.25</v>
       </c>
-      <c r="B14" s="88">
+      <c r="B14" s="87">
         <v>5.4999989999999999</v>
       </c>
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="87" t="s">
         <v>325</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="88">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="E14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="89"/>
-      <c r="M14" s="85" t="s">
+      <c r="E14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="88"/>
+      <c r="M14" s="84" t="s">
         <v>351</v>
       </c>
-      <c r="N14" s="86">
+      <c r="N14" s="85">
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A15" s="88">
+      <c r="A15" s="87">
         <v>5.5</v>
       </c>
-      <c r="B15" s="88">
+      <c r="B15" s="87">
         <v>6.4999989999999999</v>
       </c>
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="87" t="s">
         <v>324</v>
       </c>
-      <c r="D15" s="89">
+      <c r="D15" s="88">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="89"/>
-      <c r="M15" s="85" t="s">
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="88"/>
+      <c r="M15" s="84" t="s">
         <v>354</v>
       </c>
-      <c r="N15" s="86">
+      <c r="N15" s="85">
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="88">
+    <row r="16" spans="1:30" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="87">
         <v>6.5</v>
       </c>
-      <c r="B16" s="88">
+      <c r="B16" s="87">
         <v>8.4999990000000007</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="87" t="s">
         <v>323</v>
       </c>
-      <c r="D16" s="89">
+      <c r="D16" s="88">
         <v>7.7999999999999996E-3</v>
       </c>
-      <c r="E16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="89"/>
-      <c r="M16" s="85" t="s">
+      <c r="E16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="88"/>
+      <c r="M16" s="84" t="s">
         <v>353</v>
       </c>
-      <c r="N16" s="86">
+      <c r="N16" s="85">
         <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="88">
+      <c r="A17" s="87">
         <v>8.5</v>
       </c>
-      <c r="B17" s="88">
+      <c r="B17" s="87">
         <v>100000</v>
       </c>
-      <c r="C17" s="88" t="s">
+      <c r="C17" s="87" t="s">
         <v>322</v>
       </c>
-      <c r="D17" s="89">
+      <c r="D17" s="88">
         <v>6.3E-3</v>
       </c>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="89"/>
-      <c r="M17" s="85" t="s">
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="88"/>
+      <c r="M17" s="84" t="s">
         <v>356</v>
       </c>
-      <c r="N17" s="86">
+      <c r="N17" s="85">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="89"/>
-      <c r="M18" s="85" t="s">
+    <row r="18" spans="1:14" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="88"/>
+      <c r="M18" s="84" t="s">
         <v>355</v>
       </c>
-      <c r="N18" s="86">
+      <c r="N18" s="85">
         <v>2.4E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M19" s="85" t="s">
+      <c r="M19" s="84" t="s">
         <v>357</v>
       </c>
-      <c r="N19" s="86">
+      <c r="N19" s="85">
         <v>3.5099999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="85" t="s">
+    <row r="20" spans="1:14" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="84" t="s">
         <v>373</v>
       </c>
-      <c r="B20" s="88">
+      <c r="B20" s="87">
         <f>VLOOKUP("Interest Coverage",'Key Ratios'!$1:$1048576,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="88"/>
-      <c r="M20" s="85" t="s">
+      <c r="E20" s="87"/>
+      <c r="M20" s="84" t="s">
         <v>358</v>
       </c>
-      <c r="N20" s="86">
+      <c r="N20" s="85">
         <v>3.5099999999999999E-2</v>
       </c>
     </row>
@@ -13851,103 +13854,103 @@
       <c r="A21" t="s">
         <v>338</v>
       </c>
-      <c r="B21" s="66">
+      <c r="B21" s="65">
         <f>LOOKUP(B20,A3:A17,D3:D17)</f>
         <v>0.1512</v>
       </c>
-      <c r="M21" s="85" t="s">
+      <c r="M21" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="N21" s="86">
+      <c r="N21" s="85">
         <v>4.2099999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="88"/>
-      <c r="M22" s="85" t="s">
+    <row r="22" spans="1:14" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="87"/>
+      <c r="M22" s="84" t="s">
         <v>359</v>
       </c>
-      <c r="N22" s="86">
+      <c r="N22" s="85">
         <v>4.2099999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M23" s="85" t="s">
+      <c r="M23" s="84" t="s">
         <v>362</v>
       </c>
-      <c r="N23" s="86">
+      <c r="N23" s="85">
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="88"/>
-      <c r="M24" s="85" t="s">
+    <row r="24" spans="1:14" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="87"/>
+      <c r="M24" s="84" t="s">
         <v>361</v>
       </c>
-      <c r="N24" s="86">
+      <c r="N24" s="85">
         <v>5.1499999999999997E-2</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="88">
+      <c r="B25" s="87">
         <f>VLOOKUP("Interest Coverage",'Key Ratios'!$1:$1048576,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="M25" s="85" t="s">
+      <c r="M25" s="84" t="s">
         <v>363</v>
       </c>
-      <c r="N25" s="86">
+      <c r="N25" s="85">
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="88"/>
-      <c r="M26" s="85" t="s">
+    <row r="26" spans="1:14" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="87"/>
+      <c r="M26" s="84" t="s">
         <v>364</v>
       </c>
-      <c r="N26" s="86">
+      <c r="N26" s="85">
         <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M27" s="85" t="s">
+      <c r="M27" s="84" t="s">
         <v>366</v>
       </c>
-      <c r="N27" s="86">
+      <c r="N27" s="85">
         <v>8.6400000000000005E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="88"/>
-      <c r="M28" s="85" t="s">
+    <row r="28" spans="1:14" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="87"/>
+      <c r="M28" s="84" t="s">
         <v>365</v>
       </c>
-      <c r="N28" s="86">
+      <c r="N28" s="85">
         <v>8.6400000000000005E-2</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M29" s="85" t="s">
+      <c r="M29" s="84" t="s">
         <v>367</v>
       </c>
-      <c r="N29" s="86">
+      <c r="N29" s="85">
         <v>0.1134</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="85" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="88"/>
-      <c r="M30" s="85" t="s">
+    <row r="30" spans="1:14" s="84" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="87"/>
+      <c r="M30" s="84" t="s">
         <v>368</v>
       </c>
-      <c r="N30" s="86">
+      <c r="N30" s="85">
         <v>0.1134</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M31" s="85" t="s">
+      <c r="M31" s="84" t="s">
         <v>370</v>
       </c>
-      <c r="N31" s="86">
+      <c r="N31" s="85">
         <v>0.1512</v>
       </c>
     </row>
@@ -13955,7 +13958,7 @@
       <c r="M32" t="s">
         <v>369</v>
       </c>
-      <c r="N32" s="86">
+      <c r="N32" s="85">
         <v>0.1512</v>
       </c>
     </row>
@@ -13989,8 +13992,8 @@
   </sheetPr>
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14031,7 +14034,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <f>2.66 * 0</f>
+        <f>2.66 * H12</f>
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -14050,7 +14053,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f>2.66 * 0</f>
+        <f>2.66 * H12</f>
         <v>0</v>
       </c>
       <c r="C4" t="s">
@@ -14069,7 +14072,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="e">
-        <f>(H13* VLOOKUP("Stockholders' equity",'Balance Sheet (Annual)'!1:1048576,2,FALSE))/DCF!P11</f>
+        <f>(H13* VLOOKUP("Total stockholders' equity",'Balance Sheet (Annual)'!1:1048576,2,FALSE))/DCF!P11</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C5" t="s">
@@ -14106,7 +14109,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="90" t="e">
+      <c r="A7" s="89" t="e">
         <f>((H15*VLOOKUP("EBITDA",'Income Statement'!A2:AE36,2,FALSE))-H6)/DCF!P11</f>
         <v>#DIV/0!</v>
       </c>
@@ -14119,7 +14122,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G10" s="70" t="s">
+      <c r="G10" s="69" t="s">
         <v>314</v>
       </c>
     </row>
@@ -14236,10 +14239,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -14262,26 +14265,26 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="O7" s="72" t="s">
+      <c r="O7" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="P7" s="73">
+      <c r="P7" s="72">
         <f ca="1">'Growth Rates'!B1</f>
         <v>2019</v>
       </c>
-      <c r="Q7" s="73">
+      <c r="Q7" s="72">
         <f ca="1">'Growth Rates'!C1</f>
         <v>2018</v>
       </c>
-      <c r="R7" s="73">
+      <c r="R7" s="72">
         <f ca="1">'Growth Rates'!D1</f>
         <v>2017</v>
       </c>
-      <c r="S7" s="73">
+      <c r="S7" s="72">
         <f ca="1">'Growth Rates'!E1</f>
         <v>2016</v>
       </c>
-      <c r="T7" s="74">
+      <c r="T7" s="73">
         <f ca="1">'Growth Rates'!F1</f>
         <v>2015</v>
       </c>
@@ -14297,27 +14300,27 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
-      <c r="O8" s="83">
+      <c r="O8" s="82">
         <f>VLOOKUP("Dividends USD",'Key Ratios'!$1:$1048576,2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="P8" s="75">
+      <c r="P8" s="74">
         <f>VLOOKUP("Dividends USD",'Key Ratios'!$1:$1048576,3,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="75">
+      <c r="Q8" s="74">
         <f>VLOOKUP("Dividends USD",'Key Ratios'!$1:$1048576,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="75">
+      <c r="R8" s="74">
         <f>VLOOKUP("Dividends USD",'Key Ratios'!$1:$1048576,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="S8" s="75">
+      <c r="S8" s="74">
         <f>VLOOKUP("Dividends USD",'Key Ratios'!$1:$1048576,6,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="T8" s="76">
+      <c r="T8" s="75">
         <f>VLOOKUP("Dividends USD",'Key Ratios'!$1:$1048576,7,FALSE)</f>
         <v>0</v>
       </c>
@@ -14326,11 +14329,11 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="N10" s="94" t="s">
+      <c r="N10" s="93" t="s">
         <v>318</v>
       </c>
-      <c r="O10" s="95"/>
-      <c r="P10" s="96"/>
+      <c r="O10" s="94"/>
+      <c r="P10" s="95"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -14345,14 +14348,14 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="N11" s="77">
+      <c r="N11" s="76">
         <f ca="1">P7</f>
         <v>2019</v>
       </c>
       <c r="O11" t="s">
         <v>319</v>
       </c>
-      <c r="P11" s="78">
+      <c r="P11" s="77">
         <f>IFERROR((P8/T8)^(1/5)-1,0)</f>
         <v>0</v>
       </c>
@@ -14394,13 +14397,13 @@
       <c r="L12" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="79" t="s">
+      <c r="N12" s="78" t="s">
         <v>126</v>
       </c>
       <c r="O12" t="s">
         <v>319</v>
       </c>
-      <c r="P12" s="78">
+      <c r="P12" s="77">
         <f>IFERROR((O8/S8)^(1/5)-1,0)</f>
         <v>0</v>
       </c>
@@ -14453,14 +14456,14 @@
         <f>B7</f>
         <v>0</v>
       </c>
-      <c r="N13" s="77">
+      <c r="N13" s="76">
         <f ca="1">P7</f>
         <v>2019</v>
       </c>
       <c r="O13" t="s">
         <v>320</v>
       </c>
-      <c r="P13" s="78">
+      <c r="P13" s="77">
         <f>IFERROR((P8/S8)^(1/4)-1,0)</f>
         <v>0</v>
       </c>
@@ -14513,14 +14516,14 @@
         <f>(HLOOKUP(B5,B12:K14,3)*(1+L13))/(B8)</f>
         <v>#N/A</v>
       </c>
-      <c r="N14" s="77">
+      <c r="N14" s="76">
         <f ca="1">P7</f>
         <v>2019</v>
       </c>
       <c r="O14" t="s">
         <v>321</v>
       </c>
-      <c r="P14" s="78">
+      <c r="P14" s="77">
         <f>IFERROR((P8/R8)^(1/3)-1,0)</f>
         <v>0</v>
       </c>
@@ -14573,11 +14576,11 @@
         <f>L14/(1+B8)^B5</f>
         <v>#N/A</v>
       </c>
-      <c r="N15" s="80"/>
-      <c r="O15" s="81" t="s">
+      <c r="N15" s="79"/>
+      <c r="O15" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="P15" s="82" t="e">
+      <c r="P15" s="81" t="e">
         <f>AVERAGEIF(P11:P14,"&lt;&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
@@ -14605,10 +14608,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14619,32 +14622,32 @@
     <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="D1" s="97" t="s">
+      <c r="B1" s="96"/>
+      <c r="D1" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="97"/>
+      <c r="E1" s="96"/>
       <c r="I1" t="s">
         <v>61</v>
       </c>
       <c r="J1" s="23">
-        <f>VLOOKUP("Tax Rate %", 'Key Ratios'!1:1048576,2,FALSE)/100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="97" t="s">
+        <f>IF(VLOOKUP("Tax Rate %", 'Key Ratios'!1:1048576,2,FALSE) &lt; 90,VLOOKUP("Tax Rate %", 'Key Ratios'!1:1048576,2,FALSE)/100, VLOOKUP("Tax Rate %", 'Key Ratios'!1:1048576,3,FALSE))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="D3" s="97" t="s">
+      <c r="B3" s="96"/>
+      <c r="D3" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="97"/>
+      <c r="E3" s="96"/>
       <c r="I3" t="s">
         <v>63</v>
       </c>
@@ -14653,20 +14656,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="22">
         <f>VLOOKUP("Net income available to common shareholders",'Income Statement'!A2:AE36,2,FALSE)</f>
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="D4" t="s">
         <v>56</v>
       </c>
       <c r="E4">
         <f>B4</f>
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="I4" t="s">
         <v>64</v>
@@ -14676,7 +14679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -14699,7 +14702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -14715,7 +14718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -14731,7 +14734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -14749,46 +14752,49 @@
       <c r="I8" s="61" t="s">
         <v>307</v>
       </c>
-      <c r="J8" s="62">
-        <f>MIN(B9,B16,B24,B34)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J8" s="97">
+        <f t="array" ref="J8">MIN(IF(B41:B44&gt;0,B41:B44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="25">
         <f>SUM(B4:B8)</f>
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="24">
         <f>SUM(E4:E8)</f>
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="I9" s="61" t="s">
         <v>308</v>
       </c>
       <c r="J9" s="62">
-        <f>MIN(E9,E18,E24,E36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="97" t="s">
+        <f t="array" ref="J9">MIN(IF(E41:E44&gt;0,E41:E44))</f>
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="97"/>
-      <c r="D11" s="97" t="s">
+      <c r="B11" s="96"/>
+      <c r="D11" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="97"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E11" s="96"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -14804,7 +14810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -14820,7 +14826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -14836,7 +14842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -14852,7 +14858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>53</v>
       </c>
@@ -14888,14 +14894,14 @@
     </row>
     <row r="19" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="97"/>
-      <c r="D20" s="97" t="s">
+      <c r="B20" s="96"/>
+      <c r="D20" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="97"/>
+      <c r="E20" s="96"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -14963,14 +14969,14 @@
     </row>
     <row r="25" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="97" t="s">
+      <c r="A26" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="97"/>
-      <c r="D26" s="97" t="s">
+      <c r="B26" s="96"/>
+      <c r="D26" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="97"/>
+      <c r="E26" s="96"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -15009,7 +15015,7 @@
         <v>71</v>
       </c>
       <c r="B29" s="12">
-        <f>_xlfn.IFNA(VLOOKUP("Stock Compensation",'Cash Flow Statement'!1:1048576,2,FALSE),0)</f>
+        <f>_xlfn.IFNA(VLOOKUP("Stock Based Compensation",'Cash Flow Statement'!1:1048576,2,FALSE),0)</f>
         <v>0</v>
       </c>
       <c r="D29" t="s">
@@ -15119,6 +15125,70 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="21">
+        <f>B9</f>
+        <v>-1000</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41">
+        <f>E9</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="21">
+        <f>B16</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="21">
+        <f>E18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="21">
+        <f>B24</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43">
+        <f>E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="21">
+        <f>B34</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="21">
+        <f>E36</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A20:B20"/>
@@ -15161,39 +15231,39 @@
         <f ca="1">YEAR(TODAY()) - 1</f>
         <v>2019</v>
       </c>
-      <c r="C1" s="69">
+      <c r="C1" s="68">
         <f ca="1">YEAR(TODAY()) - U29</f>
         <v>2018</v>
       </c>
-      <c r="D1" s="69">
+      <c r="D1" s="68">
         <f t="shared" ref="D1:K1" ca="1" si="0">YEAR(TODAY()) - V29</f>
         <v>2017</v>
       </c>
-      <c r="E1" s="69">
+      <c r="E1" s="68">
         <f t="shared" ca="1" si="0"/>
         <v>2016</v>
       </c>
-      <c r="F1" s="69">
+      <c r="F1" s="68">
         <f t="shared" ca="1" si="0"/>
         <v>2015</v>
       </c>
-      <c r="G1" s="69">
+      <c r="G1" s="68">
         <f t="shared" ca="1" si="0"/>
         <v>2014</v>
       </c>
-      <c r="H1" s="69">
+      <c r="H1" s="68">
         <f t="shared" ca="1" si="0"/>
         <v>2013</v>
       </c>
-      <c r="I1" s="69">
+      <c r="I1" s="68">
         <f t="shared" ca="1" si="0"/>
         <v>2012</v>
       </c>
-      <c r="J1" s="69">
+      <c r="J1" s="68">
         <f t="shared" ca="1" si="0"/>
         <v>2011</v>
       </c>
-      <c r="K1" s="69">
+      <c r="K1" s="68">
         <f t="shared" ca="1" si="0"/>
         <v>2010</v>
       </c>
@@ -15982,7 +16052,7 @@
   <dimension ref="A2:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16065,52 +16135,58 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="87">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>147</v>
       </c>
@@ -16128,7 +16204,7 @@
   <dimension ref="A3:A47"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed Accrued Liability Calculation
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShyamPC\Desktop\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShyamPC\Documents\GitHub\auto-valuation-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0B3429-B4E2-4B20-A48C-AFCA53FAC7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62242CC7-C68D-4377-92F1-9EE023753C4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="6" r:id="rId1"/>
@@ -99,8 +99,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Multiples will available
-in a later update.</t>
+Will update later to use different multiples depending on industry</t>
         </r>
       </text>
     </comment>
@@ -121,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="377">
   <si>
     <t>EPS</t>
   </si>
@@ -1808,6 +1807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1829,7 +1829,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -2126,7 +2125,7 @@
   </sheetPr>
   <dimension ref="A1:AL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
@@ -2758,15 +2757,15 @@
         <v>116</v>
       </c>
       <c r="G24" s="50"/>
-      <c r="H24" s="91" t="s">
+      <c r="H24" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="91"/>
-      <c r="L24" s="91"/>
-      <c r="M24" s="91"/>
-      <c r="N24" s="91"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="92"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="92"/>
+      <c r="M24" s="92"/>
+      <c r="N24" s="92"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="33" t="s">
@@ -2783,15 +2782,15 @@
       <c r="D25" s="46">
         <v>0.8</v>
       </c>
-      <c r="H25" s="90" t="s">
+      <c r="H25" s="91" t="s">
         <v>122</v>
       </c>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="90"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="33" t="s">
@@ -2808,7 +2807,7 @@
       <c r="D26" s="46">
         <v>0.2</v>
       </c>
-      <c r="F26" s="92" t="s">
+      <c r="F26" s="93" t="s">
         <v>123</v>
       </c>
       <c r="G26" s="51" t="e">
@@ -2852,7 +2851,7 @@
       <c r="D27" s="46">
         <v>0</v>
       </c>
-      <c r="F27" s="92"/>
+      <c r="F27" s="93"/>
       <c r="G27" s="8">
         <v>5.5E-2</v>
       </c>
@@ -2895,7 +2894,7 @@
         <f>SUM(D25:D27)</f>
         <v>1</v>
       </c>
-      <c r="F28" s="92"/>
+      <c r="F28" s="93"/>
       <c r="G28" s="8">
         <v>0.06</v>
       </c>
@@ -2922,7 +2921,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="92"/>
+      <c r="F29" s="93"/>
       <c r="G29" s="8">
         <f>G28+0.005</f>
         <v>6.5000000000000002E-2</v>
@@ -2950,7 +2949,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F30" s="92"/>
+      <c r="F30" s="93"/>
       <c r="G30" s="8">
         <f t="shared" ref="G30:G33" si="3">G29+0.005</f>
         <v>7.0000000000000007E-2</v>
@@ -2978,7 +2977,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F31" s="92"/>
+      <c r="F31" s="93"/>
       <c r="G31" s="8">
         <f t="shared" si="3"/>
         <v>7.5000000000000011E-2</v>
@@ -3006,7 +3005,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F32" s="92"/>
+      <c r="F32" s="93"/>
       <c r="G32" s="8">
         <f t="shared" si="3"/>
         <v>8.0000000000000016E-2</v>
@@ -3034,7 +3033,7 @@
       </c>
     </row>
     <row r="33" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F33" s="92"/>
+      <c r="F33" s="93"/>
       <c r="G33" s="8">
         <f t="shared" si="3"/>
         <v>8.500000000000002E-2</v>
@@ -3062,7 +3061,7 @@
       </c>
     </row>
     <row r="34" spans="6:14" x14ac:dyDescent="0.3">
-      <c r="F34" s="92"/>
+      <c r="F34" s="93"/>
       <c r="G34" s="8">
         <v>0.09</v>
       </c>
@@ -13993,7 +13992,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14270,23 +14269,23 @@
       </c>
       <c r="P7" s="72">
         <f ca="1">'Growth Rates'!B1</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="Q7" s="72">
         <f ca="1">'Growth Rates'!C1</f>
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="R7" s="72">
         <f ca="1">'Growth Rates'!D1</f>
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="S7" s="72">
         <f ca="1">'Growth Rates'!E1</f>
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="T7" s="73">
         <f ca="1">'Growth Rates'!F1</f>
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14329,11 +14328,11 @@
       <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="N10" s="93" t="s">
+      <c r="N10" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="O10" s="94"/>
-      <c r="P10" s="95"/>
+      <c r="O10" s="95"/>
+      <c r="P10" s="96"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -14350,7 +14349,7 @@
       </c>
       <c r="N11" s="76">
         <f ca="1">P7</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="O11" t="s">
         <v>319</v>
@@ -14458,7 +14457,7 @@
       </c>
       <c r="N13" s="76">
         <f ca="1">P7</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="O13" t="s">
         <v>320</v>
@@ -14518,7 +14517,7 @@
       </c>
       <c r="N14" s="76">
         <f ca="1">P7</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="O14" t="s">
         <v>321</v>
@@ -14610,8 +14609,8 @@
   </sheetPr>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14623,14 +14622,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="97"/>
       <c r="I1" t="s">
         <v>61</v>
       </c>
@@ -14640,14 +14639,14 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="D3" s="96" t="s">
+      <c r="B3" s="97"/>
+      <c r="D3" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="96"/>
+      <c r="E3" s="97"/>
       <c r="I3" t="s">
         <v>63</v>
       </c>
@@ -14752,7 +14751,7 @@
       <c r="I8" s="61" t="s">
         <v>307</v>
       </c>
-      <c r="J8" s="97">
+      <c r="J8" s="90">
         <f t="array" ref="J8">MIN(IF(B41:B44&gt;0,B41:B44))</f>
         <v>0</v>
       </c>
@@ -14785,14 +14784,14 @@
     </row>
     <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="D11" s="96" t="s">
+      <c r="B11" s="97"/>
+      <c r="D11" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="96"/>
+      <c r="E11" s="97"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -14894,14 +14893,14 @@
     </row>
     <row r="19" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="96" t="s">
+      <c r="A20" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="96"/>
-      <c r="D20" s="96" t="s">
+      <c r="B20" s="97"/>
+      <c r="D20" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="96"/>
+      <c r="E20" s="97"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -14969,14 +14968,14 @@
     </row>
     <row r="25" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="96" t="s">
+      <c r="A26" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="96"/>
-      <c r="D26" s="96" t="s">
+      <c r="B26" s="97"/>
+      <c r="D26" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="96"/>
+      <c r="E26" s="97"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -15215,7 +15214,7 @@
   <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15229,43 +15228,43 @@
       </c>
       <c r="B1" s="16">
         <f ca="1">YEAR(TODAY()) - 1</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1" s="68">
         <f ca="1">YEAR(TODAY()) - U29</f>
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D1" s="68">
         <f t="shared" ref="D1:K1" ca="1" si="0">YEAR(TODAY()) - V29</f>
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E1" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F1" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="G1" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="H1" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="I1" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="J1" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="K1" s="68">
         <f t="shared" ca="1" si="0"/>
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -15802,8 +15801,11 @@
         <v>306</v>
       </c>
       <c r="B18" s="8">
-        <f>MIN(M12:M14)</f>
-        <v>0</v>
+        <f t="array" ref="B18">MIN(IF(M12:M14&gt;0,M12:M14))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="87" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
@@ -15852,7 +15854,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15972,7 +15974,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="12">
-        <f>_xlfn.IFNA(VLOOKUP(B12,'Balance Sheet (Annual)'!1:1048576,3,FALSE),0)</f>
+        <f>_xlfn.IFNA(VLOOKUP(A12,'Balance Sheet (Annual)'!1:1048576,3,FALSE),0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>